<commit_message>
Added 9 testcases, mostly related to fetch verb
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/TC_04_Create_Fetch_View.xlsx
+++ b/TestingFramework/TestData/TC_04_Create_Fetch_View.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="885" windowWidth="14805" windowHeight="7230" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="945" windowWidth="14805" windowHeight="7170" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="studiologin" sheetId="18" r:id="rId1"/>
@@ -1031,7 +1031,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>